<commit_message>
update personal info holding through upload holding section
</commit_message>
<xml_diff>
--- a/mainadminhtml/img/holding/uploadedby-Vinita_approver_userid-2.xlsx
+++ b/mainadminhtml/img/holding/uploadedby-Vinita_approver_userid-2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CBC708-AC00-4007-84AF-CDCB960907F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DC2591-9CDD-4024-B695-05C528D5FD4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,21 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>HOLDING</t>
   </si>
   <si>
     <t>PAN NO. (of all shareholders)</t>
-  </si>
-  <si>
-    <t>CBCDE1234E</t>
-  </si>
-  <si>
-    <t>ABCPE1234E</t>
-  </si>
-  <si>
-    <t>BBCPE1234E</t>
   </si>
 </sst>
 </file>
@@ -405,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,27 +416,19 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>4651561515</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3">
+        <v>1234455668</v>
       </c>
       <c r="B3">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>200</v>
+        <v>2999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>